<commit_message>
Add DC reverse ratings to production spec schottky
</commit_message>
<xml_diff>
--- a/Orbit-PCB/Elecrow/OrbitQuote.xlsx
+++ b/Orbit-PCB/Elecrow/OrbitQuote.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryota\Documents\GitHub\Orbit\Orbit-PCB\Elecrow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4B1F76D-BC07-409E-822A-9D51B3442E68}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65EC26B8-8275-4151-A6F2-ADA0C40B9618}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10680" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -227,7 +227,7 @@
       </rPr>
       <t>the component must have complete Manufacture part number</t>
     </r>
-    <phoneticPr fontId="18" type="noConversion"/>
+    <phoneticPr fontId="19" type="noConversion"/>
   </si>
   <si>
     <t>303.212 mm * 145.256 mm</t>
@@ -486,6 +486,9 @@
   </si>
   <si>
     <t>R25 R67 R87 R88</t>
+  </si>
+  <si>
+    <t>MBRX120LF-TPMSCT-ND</t>
   </si>
   <si>
     <r>
@@ -529,21 +532,35 @@
       </rPr>
       <t>1A</t>
     </r>
-  </si>
-  <si>
-    <t>MBRX120LF-TPMSCT-ND</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, DC reverse max ≥15V</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="40">
+  <fonts count="41">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1147,164 +1164,164 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1312,28 +1329,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1342,40 +1356,43 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="56">
     <cellStyle name="20% - Accent1 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
@@ -1783,10 +1800,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="23"/>
+      <c r="B1" s="22"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1909,22 +1926,22 @@
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="24"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1"/>
@@ -1939,7 +1956,7 @@
     <mergeCell ref="A13:E13"/>
     <mergeCell ref="A14:E14"/>
   </mergeCells>
-  <phoneticPr fontId="18" type="noConversion"/>
+  <phoneticPr fontId="19" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A14" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
@@ -1952,7 +1969,7 @@
   <dimension ref="A1:L49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -1962,25 +1979,25 @@
     <col min="4" max="4" width="20.26953125" customWidth="1"/>
     <col min="5" max="5" width="32" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.453125" customWidth="1"/>
-    <col min="7" max="7" width="68.08984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="71" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="4" customFormat="1" ht="25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
     </row>
     <row r="2" spans="1:12" s="4" customFormat="1" ht="14">
       <c r="A2" s="5" t="s">
@@ -2210,10 +2227,10 @@
         <v>74</v>
       </c>
       <c r="F8" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="G8" s="26" t="s">
         <v>125</v>
-      </c>
-      <c r="G8" s="22" t="s">
-        <v>124</v>
       </c>
       <c r="H8" s="5">
         <f>(2*2)</f>
@@ -2937,7 +2954,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:L1"/>
   </mergeCells>
-  <phoneticPr fontId="18" type="noConversion"/>
+  <phoneticPr fontId="19" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="L20" r:id="rId1" xr:uid="{162DF212-42AD-4C4C-A49C-669043FFA431}"/>
     <hyperlink ref="L9" r:id="rId2" xr:uid="{EE35E951-EE56-4D3B-BBA2-237225290EF4}"/>
@@ -2963,7 +2980,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="18" type="noConversion"/>
+  <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>
 </worksheet>
@@ -4438,7 +4455,7 @@
       <c r="F181" s="2"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="18" type="noConversion"/>
+  <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>
 </worksheet>

</xml_diff>